<commit_message>
fixed additional (D) and empty cols
</commit_message>
<xml_diff>
--- a/data/Election Validation/Final Sets - Clean Fixed/Governor_0622_clean_fixed.xlsx
+++ b/data/Election Validation/Final Sets - Clean Fixed/Governor_0622_clean_fixed.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdpruett/Desktop/PPRG/PPRG_R_Directory/Election Validation/Final Sets - Clean Fixed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdpruett/Desktop/CES Accuracy Analysis/data/Election Validation/Final Sets - Clean Fixed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68A4367-66B5-4348-B2E5-6EA6BF41301E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08393DD-A83E-2D4A-9C1F-15795EAAB283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="1020" windowWidth="24220" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8781" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8780" uniqueCount="1020">
   <si>
     <t>year</t>
   </si>
@@ -3093,9 +3093,6 @@
   </si>
   <si>
     <t>OtHER</t>
-  </si>
-  <si>
-    <t>added manually</t>
   </si>
 </sst>
 </file>
@@ -3448,10 +3445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z975"/>
+  <dimension ref="A1:Q975"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P243" sqref="P243"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15792,7 +15789,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="241" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>2018</v>
       </c>
@@ -15845,7 +15842,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="242" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>2018</v>
       </c>
@@ -15897,11 +15894,8 @@
       <c r="Q242" t="s">
         <v>389</v>
       </c>
-      <c r="Z242" t="s">
-        <v>1020</v>
-      </c>
-    </row>
-    <row r="243" spans="1:26" x14ac:dyDescent="0.2">
+    </row>
+    <row r="243" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>2018</v>
       </c>
@@ -15954,7 +15948,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="244" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>2018</v>
       </c>
@@ -16007,7 +16001,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="245" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>2018</v>
       </c>
@@ -16057,7 +16051,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="246" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>2018</v>
       </c>
@@ -16107,7 +16101,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="247" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>2018</v>
       </c>
@@ -16157,7 +16151,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="248" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>2018</v>
       </c>
@@ -16210,7 +16204,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="249" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>2018</v>
       </c>
@@ -16263,7 +16257,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="250" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>2018</v>
       </c>
@@ -16313,7 +16307,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="251" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>2018</v>
       </c>
@@ -16363,7 +16357,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="252" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>2018</v>
       </c>
@@ -16416,7 +16410,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="253" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>2018</v>
       </c>
@@ -16469,7 +16463,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="254" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>2018</v>
       </c>
@@ -16519,7 +16513,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="255" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>2018</v>
       </c>
@@ -16569,7 +16563,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="256" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>2018</v>
       </c>

</xml_diff>